<commit_message>
разобрал pandas.MultiIndex в pandas.Series
</commit_message>
<xml_diff>
--- a/pandas/test.xlsx
+++ b/pandas/test.xlsx
@@ -14,7 +14,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>колонки</t>
+  </si>
+  <si>
+    <t>колонка</t>
+  </si>
   <si>
     <t>col1</t>
   </si>
@@ -23,9 +32,6 @@
   </si>
   <si>
     <t>value3</t>
-  </si>
-  <si>
-    <t>code</t>
   </si>
   <si>
     <t>BLR</t>
@@ -407,52 +413,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
+      <c r="D2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -463,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -474,7 +462,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -483,7 +471,38 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>